<commit_message>
Updates, including adding the BLS data for now
</commit_message>
<xml_diff>
--- a/data/generated/job_titles.xlsx
+++ b/data/generated/job_titles.xlsx
@@ -29,31 +29,31 @@
     <t>Administrative Staff</t>
   </si>
   <si>
-    <t>Senior Staff</t>
-  </si>
-  <si>
-    <t>Archivist</t>
-  </si>
-  <si>
-    <t>Curator</t>
-  </si>
-  <si>
-    <t>Data Librarian</t>
-  </si>
-  <si>
-    <t>Scientist</t>
-  </si>
-  <si>
-    <t>Policy Specialist</t>
-  </si>
-  <si>
-    <t>Project Manager</t>
-  </si>
-  <si>
-    <t>Researcher</t>
-  </si>
-  <si>
-    <t>Software Engineer</t>
+    <t>Archivists</t>
+  </si>
+  <si>
+    <t>Curators</t>
+  </si>
+  <si>
+    <t>Data Librarians</t>
+  </si>
+  <si>
+    <t>Scientists</t>
+  </si>
+  <si>
+    <t>Policy Specialists</t>
+  </si>
+  <si>
+    <t>Project Managers</t>
+  </si>
+  <si>
+    <t>Researchers</t>
+  </si>
+  <si>
+    <t>Senior Staffs</t>
+  </si>
+  <si>
+    <t>Software Engineers</t>
   </si>
 </sst>
 </file>
@@ -413,42 +413,42 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="26" x14ac:dyDescent="0.35">

</xml_diff>